<commit_message>
KORQuAD & SQuAD Benchmark Charts
</commit_message>
<xml_diff>
--- a/Results/Experiments_Results.xlsx
+++ b/Results/Experiments_Results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\masters-research-qa\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D42BF20-1485-4701-A028-EBF329B2349A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77516E7-D276-42F2-AC88-F7B892EFA738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MLQA" sheetId="1" r:id="rId1"/>
     <sheet name="XQuAD" sheetId="2" r:id="rId2"/>
     <sheet name="SQuAD-IT" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="KORQuAD" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MLQA!$A$76:$S$76</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="56">
   <si>
     <t>hi</t>
   </si>
@@ -200,6 +201,15 @@
   </si>
   <si>
     <t>KD-ES</t>
+  </si>
+  <si>
+    <t>SQuAD-IT</t>
+  </si>
+  <si>
+    <t>KORQuAD</t>
+  </si>
+  <si>
+    <t>KD-ZH</t>
   </si>
 </sst>
 </file>
@@ -594,6 +604,15 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -601,15 +620,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4785,7 +4795,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-IN" baseline="0"/>
-              <a:t> Benchmark</a:t>
+              <a:t> Benchmarks</a:t>
             </a:r>
             <a:endParaRPr lang="en-IN"/>
           </a:p>
@@ -4886,6 +4896,62 @@
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'SQuAD-IT'!$A$3:$A$6</c:f>
@@ -4986,6 +5052,62 @@
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'SQuAD-IT'!$A$3:$A$6</c:f>
@@ -5034,8 +5156,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -5053,6 +5176,59 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Model TRAINED on LANGUAGE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5117,6 +5293,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Scores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5148,6 +5377,705 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1928393839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>KORQuAD Benchmarks</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>KORQuAD!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>KORQuAD!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KD-EN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KD-ZH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>KORQuAD!$B$3:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>51.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-65AC-40C8-B230-F436EC2665AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>KORQuAD!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>KORQuAD!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KD-EN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KD-ZH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>KORQuAD!$C$3:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>61.82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69.040000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-65AC-40C8-B230-F436EC2665AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="1121854016"/>
+        <c:axId val="1121839040"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1121854016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>model trained on language</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1121839040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1121839040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>scores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1121854016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15312,6 +16240,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -16642,6 +17610,502 @@
 </file>
 
 <file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -21602,16 +23066,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>450532</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>16192</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>325755</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>92393</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>501015</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>16193</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -21619,6 +23083,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD0416EE-8438-4E17-9666-D1FBD8AAB495}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDFCCD7A-0AEA-4B05-9A2A-21F3669AF414}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -22082,27 +23587,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -22127,29 +23632,29 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -22614,27 +24119,27 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
     </row>
     <row r="19" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
@@ -22659,29 +24164,29 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="37" t="s">
+      <c r="K24" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="37"/>
-      <c r="S24" s="37"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
@@ -22976,27 +24481,27 @@
       <c r="S32" s="10"/>
     </row>
     <row r="35" spans="1:19" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="35"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="35"/>
-      <c r="O35" s="35"/>
-      <c r="P35" s="35"/>
-      <c r="Q35" s="35"/>
-      <c r="R35" s="35"/>
-      <c r="S35" s="35"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="34"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="34"/>
+      <c r="P35" s="34"/>
+      <c r="Q35" s="34"/>
+      <c r="R35" s="34"/>
+      <c r="S35" s="34"/>
     </row>
     <row r="36" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
@@ -23016,29 +24521,29 @@
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="37" t="s">
+      <c r="K41" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="L41" s="37"/>
-      <c r="M41" s="37"/>
-      <c r="N41" s="37"/>
-      <c r="O41" s="37"/>
-      <c r="P41" s="37"/>
-      <c r="Q41" s="37"/>
-      <c r="R41" s="37"/>
-      <c r="S41" s="37"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+      <c r="S41" s="33"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
@@ -23503,27 +25008,27 @@
       </c>
     </row>
     <row r="52" spans="1:19" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="35"/>
-      <c r="J52" s="35"/>
-      <c r="K52" s="35"/>
-      <c r="L52" s="35"/>
-      <c r="M52" s="35"/>
-      <c r="N52" s="35"/>
-      <c r="O52" s="35"/>
-      <c r="P52" s="35"/>
-      <c r="Q52" s="35"/>
-      <c r="R52" s="35"/>
-      <c r="S52" s="35"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="34"/>
+      <c r="K52" s="34"/>
+      <c r="L52" s="34"/>
+      <c r="M52" s="34"/>
+      <c r="N52" s="34"/>
+      <c r="O52" s="34"/>
+      <c r="P52" s="34"/>
+      <c r="Q52" s="34"/>
+      <c r="R52" s="34"/>
+      <c r="S52" s="34"/>
     </row>
     <row r="53" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
@@ -23543,29 +25048,29 @@
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A58" s="36" t="s">
+      <c r="A58" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="36"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
       <c r="J58" s="2"/>
-      <c r="K58" s="37" t="s">
+      <c r="K58" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="L58" s="37"/>
-      <c r="M58" s="37"/>
-      <c r="N58" s="37"/>
-      <c r="O58" s="37"/>
-      <c r="P58" s="37"/>
-      <c r="Q58" s="37"/>
-      <c r="R58" s="37"/>
-      <c r="S58" s="37"/>
+      <c r="L58" s="33"/>
+      <c r="M58" s="33"/>
+      <c r="N58" s="33"/>
+      <c r="O58" s="33"/>
+      <c r="P58" s="33"/>
+      <c r="Q58" s="33"/>
+      <c r="R58" s="33"/>
+      <c r="S58" s="33"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
@@ -23836,27 +25341,27 @@
       </c>
     </row>
     <row r="69" spans="1:20" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="32" t="s">
+      <c r="A69" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B69" s="32"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="32"/>
-      <c r="H69" s="32"/>
-      <c r="I69" s="32"/>
-      <c r="J69" s="32"/>
-      <c r="K69" s="32"/>
-      <c r="L69" s="32"/>
-      <c r="M69" s="32"/>
-      <c r="N69" s="32"/>
-      <c r="O69" s="32"/>
-      <c r="P69" s="32"/>
-      <c r="Q69" s="32"/>
-      <c r="R69" s="32"/>
-      <c r="S69" s="32"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="35"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="35"/>
+      <c r="H69" s="35"/>
+      <c r="I69" s="35"/>
+      <c r="J69" s="35"/>
+      <c r="K69" s="35"/>
+      <c r="L69" s="35"/>
+      <c r="M69" s="35"/>
+      <c r="N69" s="35"/>
+      <c r="O69" s="35"/>
+      <c r="P69" s="35"/>
+      <c r="Q69" s="35"/>
+      <c r="R69" s="35"/>
+      <c r="S69" s="35"/>
     </row>
     <row r="70" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A70" s="11"/>
@@ -23972,29 +25477,29 @@
       <c r="S74" s="11"/>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A75" s="33" t="s">
+      <c r="A75" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B75" s="33"/>
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="33"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="33"/>
-      <c r="H75" s="33"/>
-      <c r="I75" s="33"/>
+      <c r="B75" s="36"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="36"/>
+      <c r="I75" s="36"/>
       <c r="J75" s="12"/>
-      <c r="K75" s="34" t="s">
+      <c r="K75" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="L75" s="34"/>
-      <c r="M75" s="34"/>
-      <c r="N75" s="34"/>
-      <c r="O75" s="34"/>
-      <c r="P75" s="34"/>
-      <c r="Q75" s="34"/>
-      <c r="R75" s="34"/>
-      <c r="S75" s="34"/>
+      <c r="L75" s="37"/>
+      <c r="M75" s="37"/>
+      <c r="N75" s="37"/>
+      <c r="O75" s="37"/>
+      <c r="P75" s="37"/>
+      <c r="Q75" s="37"/>
+      <c r="R75" s="37"/>
+      <c r="S75" s="37"/>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" s="19" t="s">
@@ -24491,27 +25996,27 @@
       </c>
     </row>
     <row r="86" spans="1:20" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="32" t="s">
+      <c r="A86" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B86" s="32"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="32"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="32"/>
-      <c r="G86" s="32"/>
-      <c r="H86" s="32"/>
-      <c r="I86" s="32"/>
-      <c r="J86" s="32"/>
-      <c r="K86" s="32"/>
-      <c r="L86" s="32"/>
-      <c r="M86" s="32"/>
-      <c r="N86" s="32"/>
-      <c r="O86" s="32"/>
-      <c r="P86" s="32"/>
-      <c r="Q86" s="32"/>
-      <c r="R86" s="32"/>
-      <c r="S86" s="32"/>
+      <c r="B86" s="35"/>
+      <c r="C86" s="35"/>
+      <c r="D86" s="35"/>
+      <c r="E86" s="35"/>
+      <c r="F86" s="35"/>
+      <c r="G86" s="35"/>
+      <c r="H86" s="35"/>
+      <c r="I86" s="35"/>
+      <c r="J86" s="35"/>
+      <c r="K86" s="35"/>
+      <c r="L86" s="35"/>
+      <c r="M86" s="35"/>
+      <c r="N86" s="35"/>
+      <c r="O86" s="35"/>
+      <c r="P86" s="35"/>
+      <c r="Q86" s="35"/>
+      <c r="R86" s="35"/>
+      <c r="S86" s="35"/>
     </row>
     <row r="87" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A87" s="11"/>
@@ -24627,29 +26132,29 @@
       <c r="S91" s="11"/>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A92" s="33" t="s">
+      <c r="A92" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B92" s="33"/>
-      <c r="C92" s="33"/>
-      <c r="D92" s="33"/>
-      <c r="E92" s="33"/>
-      <c r="F92" s="33"/>
-      <c r="G92" s="33"/>
-      <c r="H92" s="33"/>
-      <c r="I92" s="33"/>
+      <c r="B92" s="36"/>
+      <c r="C92" s="36"/>
+      <c r="D92" s="36"/>
+      <c r="E92" s="36"/>
+      <c r="F92" s="36"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="36"/>
+      <c r="I92" s="36"/>
       <c r="J92" s="12"/>
-      <c r="K92" s="34" t="s">
+      <c r="K92" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="L92" s="34"/>
-      <c r="M92" s="34"/>
-      <c r="N92" s="34"/>
-      <c r="O92" s="34"/>
-      <c r="P92" s="34"/>
-      <c r="Q92" s="34"/>
-      <c r="R92" s="34"/>
-      <c r="S92" s="34"/>
+      <c r="L92" s="37"/>
+      <c r="M92" s="37"/>
+      <c r="N92" s="37"/>
+      <c r="O92" s="37"/>
+      <c r="P92" s="37"/>
+      <c r="Q92" s="37"/>
+      <c r="R92" s="37"/>
+      <c r="S92" s="37"/>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" s="19" t="s">
@@ -24987,24 +26492,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A86:S86"/>
+    <mergeCell ref="A92:I92"/>
+    <mergeCell ref="K92:S92"/>
+    <mergeCell ref="A69:S69"/>
+    <mergeCell ref="A75:I75"/>
+    <mergeCell ref="K75:S75"/>
+    <mergeCell ref="A35:S35"/>
+    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="K41:S41"/>
+    <mergeCell ref="A52:S52"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="K58:S58"/>
     <mergeCell ref="A7:I7"/>
     <mergeCell ref="K7:S7"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A18:S18"/>
     <mergeCell ref="A24:I24"/>
     <mergeCell ref="K24:S24"/>
-    <mergeCell ref="A35:S35"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="K41:S41"/>
-    <mergeCell ref="A52:S52"/>
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="K58:S58"/>
-    <mergeCell ref="A86:S86"/>
-    <mergeCell ref="A92:I92"/>
-    <mergeCell ref="K92:S92"/>
-    <mergeCell ref="A69:S69"/>
-    <mergeCell ref="A75:I75"/>
-    <mergeCell ref="K75:S75"/>
   </mergeCells>
   <conditionalFormatting sqref="L9:R15">
     <cfRule type="colorScale" priority="36">
@@ -25421,28 +26926,28 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="K5" s="34" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="K5" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
@@ -25759,37 +27264,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7FCD4-2E60-4AB1-975A-95BC4C49F966}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
@@ -25805,17 +27301,8 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>39</v>
       </c>
@@ -25831,17 +27318,8 @@
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>49</v>
       </c>
@@ -25857,17 +27335,8 @@
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>52</v>
       </c>
@@ -25883,17 +27352,8 @@
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>50</v>
       </c>
@@ -25909,45 +27369,11 @@
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
       <c r="I6" s="17"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="K1:S1"/>
   </mergeCells>
-  <conditionalFormatting sqref="K4:K5">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K6">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A3:B5 I6 D3:I5">
     <cfRule type="colorScale" priority="5">
       <colorScale>
@@ -25962,30 +27388,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B6 D6:H6">
     <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:S3 S6 L4:S5">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L6:R6">
-    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -26026,11 +27428,135 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0482654-746B-41F0-B950-3A7AA7600544}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="17">
+        <v>51.51</v>
+      </c>
+      <c r="C3" s="17">
+        <v>61.82</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="17">
+        <v>54.12</v>
+      </c>
+      <c r="C4" s="17">
+        <v>64.63</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="17">
+        <v>58.43</v>
+      </c>
+      <c r="C5" s="17">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C3:C5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:B5 D3:I5">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E210D27-1723-47AE-8660-08824278ACBC}">
   <dimension ref="A5:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>